<commit_message>
jenkins run code change
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divakarab\IdeaProjects\TestNGNEW\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8773D423-1A7D-44D0-B453-F43CB1CE551F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A271C75-D466-47C7-8311-2246D5CCD973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFCD890B-1D0D-4C44-BE0C-1E139FBC73C1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>